<commit_message>
adicionando o script do corte das camadas ambientais futuras
</commit_message>
<xml_diff>
--- a/Cronograma_atividades.xlsx
+++ b/Cronograma_atividades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guich\Documents\PDPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BECFF8-D588-40D7-A167-00F3E6EBD1A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F085E89E-876C-499C-9F2D-E7AC90739172}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,7 +339,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +355,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -407,6 +413,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,7 +635,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -829,8 +836,8 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>

</xml_diff>